<commit_message>
Wrote and passed tests for the sending and receving of the messages. Validating a lot of functionality
Detected an corrected an error when expanding multiplexed signals
Also detected an error when packing and unpacking signals with double and single datatypes but it is not solved YET!
</commit_message>
<xml_diff>
--- a/test/FeaturesTestMatrix.xlsx
+++ b/test/FeaturesTestMatrix.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/50baad01ae7f11f1/Electronica/CANDatabaseLayer/CANDatabaseLayer/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="806" documentId="8_{601BBFC0-121C-4D4C-831B-4E3A07B6196F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2F32F590-AD27-487F-87DE-E6056EFB1DB4}"/>
+  <xr:revisionPtr revIDLastSave="1183" documentId="8_{601BBFC0-121C-4D4C-831B-4E3A07B6196F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E5A38404-80D1-466D-8CF8-2B5FD329738A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{CF8A19B2-AC85-44D0-8427-F34C59F4D7C2}"/>
+    <workbookView xWindow="28680" yWindow="1245" windowWidth="19440" windowHeight="15150" activeTab="1" xr2:uid="{CF8A19B2-AC85-44D0-8427-F34C59F4D7C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="134">
   <si>
     <t>Messages</t>
   </si>
@@ -256,13 +257,193 @@
   </si>
   <si>
     <t>Signal getValue</t>
+  </si>
+  <si>
+    <t>Example 1</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Example 2</t>
+  </si>
+  <si>
+    <t>Example 3</t>
+  </si>
+  <si>
+    <t>Example 4</t>
+  </si>
+  <si>
+    <t>Transmit/Receive</t>
+  </si>
+  <si>
+    <t>-2.138737678527832</t>
+  </si>
+  <si>
+    <t>-8.984071263822772e-28</t>
+  </si>
+  <si>
+    <t>210101152.0</t>
+  </si>
+  <si>
+    <t>1.933080063378043e-17</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>-23</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>48009</t>
+  </si>
+  <si>
+    <t>115</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>-4215</t>
+  </si>
+  <si>
+    <t>239</t>
+  </si>
+  <si>
+    <t>167</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>12898</t>
+  </si>
+  <si>
+    <t>57288</t>
+  </si>
+  <si>
+    <t>-13</t>
+  </si>
+  <si>
+    <t>217</t>
+  </si>
+  <si>
+    <t>216</t>
+  </si>
+  <si>
+    <t>31189</t>
+  </si>
+  <si>
+    <t>42039</t>
+  </si>
+  <si>
+    <t>375</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>0x0000e299008a00e6</t>
+  </si>
+  <si>
+    <t>0x0000169900a705de</t>
+  </si>
+  <si>
+    <t>0x54603262d912dfc8</t>
+  </si>
+  <si>
+    <t>0x927ca43738a679d5</t>
+  </si>
+  <si>
+    <t>0x0000000000000082</t>
+  </si>
+  <si>
+    <t>0x0000000000000074</t>
+  </si>
+  <si>
+    <t>0x0000000000000046</t>
+  </si>
+  <si>
+    <t>0x0000000000000043</t>
+  </si>
+  <si>
+    <t>0x0000000000001784</t>
+  </si>
+  <si>
+    <t>0x0000000000009d31</t>
+  </si>
+  <si>
+    <t>0xe797a6e9c062d900</t>
+  </si>
+  <si>
+    <t>0xb1e1e4eb60af8201</t>
+  </si>
+  <si>
+    <t>0x7e0868676c2b0004</t>
+  </si>
+  <si>
+    <t>0xe74aa821e19e0104</t>
+  </si>
+  <si>
+    <t>0x0000000000250000</t>
+  </si>
+  <si>
+    <t>0x0000000000000001</t>
+  </si>
+  <si>
+    <t>0x0000000000000000</t>
+  </si>
+  <si>
+    <t>0x0000000000001000</t>
+  </si>
+  <si>
+    <t>0xb95b8e92c008e114</t>
+  </si>
+  <si>
+    <t>0x904bb2234d485e3a</t>
+  </si>
+  <si>
+    <t>0x4e46c7d11d92219d</t>
+  </si>
+  <si>
+    <t>0x95b33faa5b14009a</t>
+  </si>
+  <si>
+    <t>0x0000000000000044</t>
+  </si>
+  <si>
+    <t>0x0000000000000036</t>
+  </si>
+  <si>
+    <t>1.22832399570192E+85</t>
+  </si>
+  <si>
+    <t>-3.83710954814724E-189</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,6 +455,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -339,7 +526,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -374,531 +561,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="66">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <font>
         <color theme="0"/>
@@ -1356,11 +1030,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4D89094-6B54-475A-BA41-6FD743780258}">
   <dimension ref="A1:AD77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2:I2"/>
+      <selection pane="bottomRight" activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3485,6 +3159,9 @@
       <c r="A42" s="15" t="s">
         <v>67</v>
       </c>
+      <c r="D42" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="O42" s="1"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
@@ -3729,7 +3406,7 @@
       </c>
       <c r="D51" s="1">
         <f t="shared" ref="D51:X51" si="0">COUNTIF(D4:D49,TRUE)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E51" s="1">
         <f t="shared" si="0"/>
@@ -4163,62 +3840,672 @@
     <mergeCell ref="L2:P2"/>
   </mergeCells>
   <conditionalFormatting sqref="J4:J52">
-    <cfRule type="cellIs" dxfId="65" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="55" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="56" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51:AD52 AD37 AD23 AD17:AD18 AD9:AD12 AD7 C4:AB50">
-    <cfRule type="cellIs" dxfId="1" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="57" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="58" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD36">
-    <cfRule type="cellIs" dxfId="63" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="53" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="54" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD5">
-    <cfRule type="cellIs" dxfId="61" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="51" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="52" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC26">
-    <cfRule type="cellIs" dxfId="57" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC4:AC23 AC25 AC27:AC50">
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC24">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C909A9B3-3389-4B5C-A3B0-49ED15F847B8}">
+  <dimension ref="A2:K43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" style="22" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="22"/>
+    <col min="6" max="6" width="12.42578125" style="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>Matrix!A3</f>
+        <v>Messages</v>
+      </c>
+      <c r="B3" t="str">
+        <f>Matrix!B3</f>
+        <v>Signals</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f>Matrix!A4</f>
+        <v>ABSdata (0xC9)</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" t="str">
+        <f>Matrix!B5</f>
+        <v>AccelerationForce</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" t="str">
+        <f>Matrix!B6</f>
+        <v>Diagnostics</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" t="str">
+        <f>Matrix!B7</f>
+        <v>GearLock</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B8" t="str">
+        <f>Matrix!B8</f>
+        <v>CarSpeed</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f>Matrix!A9</f>
+        <v>EngineData (0x64)</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" t="str">
+        <f>Matrix!B10</f>
+        <v>EngSpeed</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" t="str">
+        <f>Matrix!B11</f>
+        <v>EngTemp</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" t="str">
+        <f>Matrix!B12</f>
+        <v>IdleRunning</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" t="str">
+        <f>Matrix!B13</f>
+        <v>EngForce</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" t="str">
+        <f>Matrix!B14</f>
+        <v>EngPower</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" t="str">
+        <f>Matrix!B15</f>
+        <v>PetrolLevel</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f>Matrix!A16</f>
+        <v>EngineStatus (0x65)</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B17" t="str">
+        <f>Matrix!B17</f>
+        <v>Status</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B18" t="str">
+        <f>Matrix!B18</f>
+        <v>ErrorCode</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f>Matrix!A19</f>
+        <v>GearboxInfo (0x3FC)</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="H19" t="s">
+        <v>114</v>
+      </c>
+      <c r="J19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B20" t="str">
+        <f>Matrix!B20</f>
+        <v>Gear</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="H20">
+        <v>3</v>
+      </c>
+      <c r="J20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B21" t="str">
+        <f>Matrix!B21</f>
+        <v>ShiftRequest</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B22" t="str">
+        <f>Matrix!B22</f>
+        <v>EcoMode</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B23" t="str">
+        <f>Matrix!B23</f>
+        <v>GearLock</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f>Matrix!A24</f>
+        <v>Ignition_Info (0x67)</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B25" t="str">
+        <f>Matrix!B25</f>
+        <v>StarterKey</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f>Matrix!A26</f>
+        <v>MultiplexExample (0x300)</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="H26" t="s">
+        <v>120</v>
+      </c>
+      <c r="J26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B27" t="str">
+        <f>Matrix!B27</f>
+        <v>ExSignal1</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="F27" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="H27">
+        <v>4</v>
+      </c>
+      <c r="J27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B28" t="str">
+        <f>Matrix!B28</f>
+        <v>ExSignal2</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B29" t="str">
+        <f>Matrix!B29</f>
+        <v>ExSignal3</v>
+      </c>
+      <c r="H29">
+        <v>43</v>
+      </c>
+      <c r="J29">
+        <v>-98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B30" t="str">
+        <f>Matrix!B30</f>
+        <v>ExSignal4</v>
+      </c>
+      <c r="H30">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B31" t="str">
+        <f>Matrix!B31</f>
+        <v>ExSignal5</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B32" t="str">
+        <f>Matrix!B32</f>
+        <v>ExSignal6</v>
+      </c>
+      <c r="H32">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="str">
+        <f>Matrix!A33</f>
+        <v>MultiplexExample2 (0x301)</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="F33" s="22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B34" t="str">
+        <f>Matrix!B34</f>
+        <v>ExSignal7</v>
+      </c>
+      <c r="D34" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="F34" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B35" t="str">
+        <f>Matrix!B35</f>
+        <v>ExSignal8</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="F35" s="22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B36" t="str">
+        <f>Matrix!B36</f>
+        <v>ExSignal9</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="F36" s="22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="str">
+        <f>Matrix!A37</f>
+        <v>NM_Engine (0x51B)</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="F37" s="22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B38" t="str">
+        <f>Matrix!B38</f>
+        <v>SleepInd</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="F38" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="str">
+        <f>Matrix!A39</f>
+        <v>FloatExample (0xC01FEFE)</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="F39" s="22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B40" t="str">
+        <f>Matrix!B40</f>
+        <v>SingleExample</v>
+      </c>
+      <c r="D40" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="F40" s="22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B41" t="str">
+        <f>Matrix!B41</f>
+        <v>SingleExample2</v>
+      </c>
+      <c r="D41" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="F41" s="22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="str">
+        <f>Matrix!A42</f>
+        <v>FloatExample2 (0x301)</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="F42" s="22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B43" t="str">
+        <f>Matrix!B43</f>
+        <v>DoubleExample</v>
+      </c>
+      <c r="D43" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="F43" s="22" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Big redo on the raw message datatype. I was using a unique uint64_t that was taking a lot of space for small messages and didn't allow bigger messages for the future CANFD extension. Now all messages have a list of union with an array of bytes with the length of the DLC. This union also contains structures with padding and the raw signal that are used by the receive and send methods. These now are suuuupersimple and elegant :). Redone validation on the test project and seems to be working fine
</commit_message>
<xml_diff>
--- a/test/FeaturesTestMatrix.xlsx
+++ b/test/FeaturesTestMatrix.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/50baad01ae7f11f1/Electronica/CANDatabaseLayer/CANDatabaseLayer/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/50baad01ae7f11f1/Altran/ICURepo/Comms/cantata/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1183" documentId="8_{601BBFC0-121C-4D4C-831B-4E3A07B6196F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E5A38404-80D1-466D-8CF8-2B5FD329738A}"/>
@@ -552,6 +552,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -561,13 +568,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1061,42 +1061,42 @@
     </row>
     <row r="2" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="13"/>
-      <c r="C2" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
+      <c r="C2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
       <c r="J2" s="10"/>
       <c r="K2" s="12"/>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="17" t="s">
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="18"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="17" t="s">
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="21"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="21"/>
+      <c r="X2" s="22"/>
+      <c r="Y2" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="Z2" s="18"/>
-      <c r="AA2" s="18"/>
-      <c r="AB2" s="18"/>
-      <c r="AC2" s="18"/>
-      <c r="AD2" s="18"/>
+      <c r="Z2" s="21"/>
+      <c r="AA2" s="21"/>
+      <c r="AB2" s="21"/>
+      <c r="AC2" s="21"/>
+      <c r="AD2" s="21"/>
     </row>
     <row r="3" spans="1:30" s="3" customFormat="1" ht="172.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -3905,10 +3905,10 @@
   <dimension ref="A2:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
+      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3916,37 +3916,37 @@
     <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="30.85546875" style="22" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="22"/>
-    <col min="6" max="6" width="12.42578125" style="22" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" style="19" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="19"/>
+    <col min="6" max="6" width="12.42578125" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="17" t="s">
         <v>75</v>
       </c>
     </row>
@@ -3968,10 +3968,10 @@
       <c r="C4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="19" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3980,10 +3980,10 @@
         <f>Matrix!B5</f>
         <v>AccelerationForce</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="19" t="s">
         <v>93</v>
       </c>
     </row>
@@ -3992,10 +3992,10 @@
         <f>Matrix!B6</f>
         <v>Diagnostics</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="19" t="s">
         <v>95</v>
       </c>
     </row>
@@ -4004,10 +4004,10 @@
         <f>Matrix!B7</f>
         <v>GearLock</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="19" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4016,10 +4016,10 @@
         <f>Matrix!B8</f>
         <v>CarSpeed</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="19" t="s">
         <v>94</v>
       </c>
     </row>
@@ -4031,10 +4031,10 @@
       <c r="C9" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="19" t="s">
         <v>111</v>
       </c>
     </row>
@@ -4043,10 +4043,10 @@
         <f>Matrix!B10</f>
         <v>EngSpeed</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="19" t="s">
         <v>104</v>
       </c>
     </row>
@@ -4055,10 +4055,10 @@
         <f>Matrix!B11</f>
         <v>EngTemp</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="19" t="s">
         <v>87</v>
       </c>
     </row>
@@ -4067,10 +4067,10 @@
         <f>Matrix!B12</f>
         <v>IdleRunning</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="19" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4079,10 +4079,10 @@
         <f>Matrix!B13</f>
         <v>EngForce</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="19" t="s">
         <v>105</v>
       </c>
     </row>
@@ -4091,10 +4091,10 @@
         <f>Matrix!B14</f>
         <v>EngPower</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="F14" s="19" t="s">
         <v>106</v>
       </c>
     </row>
@@ -4103,10 +4103,10 @@
         <f>Matrix!B15</f>
         <v>PetrolLevel</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="19" t="s">
         <v>107</v>
       </c>
     </row>
@@ -4118,10 +4118,10 @@
       <c r="C16" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="F16" s="19" t="s">
         <v>113</v>
       </c>
     </row>
@@ -4130,10 +4130,10 @@
         <f>Matrix!B17</f>
         <v>Status</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="F17" s="19" t="s">
         <v>84</v>
       </c>
     </row>
@@ -4142,10 +4142,10 @@
         <f>Matrix!B18</f>
         <v>ErrorCode</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="19" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4157,10 +4157,10 @@
       <c r="C19" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="F19" s="22" t="s">
+      <c r="F19" s="19" t="s">
         <v>130</v>
       </c>
       <c r="H19" t="s">
@@ -4175,10 +4175,10 @@
         <f>Matrix!B20</f>
         <v>Gear</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D20" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="F20" s="22" t="s">
+      <c r="F20" s="19" t="s">
         <v>85</v>
       </c>
       <c r="H20">
@@ -4193,10 +4193,10 @@
         <f>Matrix!B21</f>
         <v>ShiftRequest</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="F21" s="22" t="s">
+      <c r="F21" s="19" t="s">
         <v>84</v>
       </c>
       <c r="H21">
@@ -4211,10 +4211,10 @@
         <f>Matrix!B22</f>
         <v>EcoMode</v>
       </c>
-      <c r="D22" s="22" t="s">
+      <c r="D22" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="F22" s="22" t="s">
+      <c r="F22" s="19" t="s">
         <v>85</v>
       </c>
       <c r="H22">
@@ -4229,10 +4229,10 @@
         <f>Matrix!B23</f>
         <v>GearLock</v>
       </c>
-      <c r="D23" s="22" t="s">
+      <c r="D23" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="F23" s="22" t="s">
+      <c r="F23" s="19" t="s">
         <v>84</v>
       </c>
       <c r="H23">
@@ -4250,10 +4250,10 @@
       <c r="C24" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D24" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="F24" s="22" t="s">
+      <c r="F24" s="19" t="s">
         <v>117</v>
       </c>
     </row>
@@ -4262,10 +4262,10 @@
         <f>Matrix!B25</f>
         <v>StarterKey</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="F25" s="22" t="s">
+      <c r="F25" s="19" t="s">
         <v>84</v>
       </c>
     </row>
@@ -4277,10 +4277,10 @@
       <c r="C26" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="22" t="s">
+      <c r="D26" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="F26" s="22" t="s">
+      <c r="F26" s="19" t="s">
         <v>119</v>
       </c>
       <c r="H26" t="s">
@@ -4295,10 +4295,10 @@
         <f>Matrix!B27</f>
         <v>ExSignal1</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="F27" s="22" t="s">
+      <c r="F27" s="19" t="s">
         <v>85</v>
       </c>
       <c r="H27">
@@ -4346,7 +4346,7 @@
         <f>Matrix!B31</f>
         <v>ExSignal5</v>
       </c>
-      <c r="D31" s="22" t="s">
+      <c r="D31" s="19" t="s">
         <v>86</v>
       </c>
     </row>
@@ -4367,10 +4367,10 @@
       <c r="C33" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D33" s="22" t="s">
+      <c r="D33" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="F33" s="22" t="s">
+      <c r="F33" s="19" t="s">
         <v>123</v>
       </c>
     </row>
@@ -4379,10 +4379,10 @@
         <f>Matrix!B34</f>
         <v>ExSignal7</v>
       </c>
-      <c r="D34" s="22" t="s">
+      <c r="D34" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="F34" s="22" t="s">
+      <c r="F34" s="19" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4391,10 +4391,10 @@
         <f>Matrix!B35</f>
         <v>ExSignal8</v>
       </c>
-      <c r="D35" s="22" t="s">
+      <c r="D35" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="F35" s="22" t="s">
+      <c r="F35" s="19" t="s">
         <v>84</v>
       </c>
     </row>
@@ -4403,10 +4403,10 @@
         <f>Matrix!B36</f>
         <v>ExSignal9</v>
       </c>
-      <c r="D36" s="22" t="s">
+      <c r="D36" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="F36" s="22" t="s">
+      <c r="F36" s="19" t="s">
         <v>84</v>
       </c>
     </row>
@@ -4418,10 +4418,10 @@
       <c r="C37" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D37" s="22" t="s">
+      <c r="D37" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="F37" s="22" t="s">
+      <c r="F37" s="19" t="s">
         <v>125</v>
       </c>
     </row>
@@ -4430,10 +4430,10 @@
         <f>Matrix!B38</f>
         <v>SleepInd</v>
       </c>
-      <c r="D38" s="22" t="s">
+      <c r="D38" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="F38" s="22" t="s">
+      <c r="F38" s="19" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4445,10 +4445,10 @@
       <c r="C39" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D39" s="22" t="s">
+      <c r="D39" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="F39" s="22" t="s">
+      <c r="F39" s="19" t="s">
         <v>127</v>
       </c>
     </row>
@@ -4457,10 +4457,10 @@
         <f>Matrix!B40</f>
         <v>SingleExample</v>
       </c>
-      <c r="D40" s="22" t="s">
+      <c r="D40" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="F40" s="22" t="s">
+      <c r="F40" s="19" t="s">
         <v>82</v>
       </c>
     </row>
@@ -4469,10 +4469,10 @@
         <f>Matrix!B41</f>
         <v>SingleExample2</v>
       </c>
-      <c r="D41" s="22" t="s">
+      <c r="D41" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="F41" s="22" t="s">
+      <c r="F41" s="19" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4484,10 +4484,10 @@
       <c r="C42" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D42" s="22" t="s">
+      <c r="D42" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="F42" s="22" t="s">
+      <c r="F42" s="19" t="s">
         <v>129</v>
       </c>
     </row>
@@ -4496,10 +4496,10 @@
         <f>Matrix!B43</f>
         <v>DoubleExample</v>
       </c>
-      <c r="D43" s="22" t="s">
+      <c r="D43" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="F43" s="22" t="s">
+      <c r="F43" s="19" t="s">
         <v>133</v>
       </c>
     </row>

</xml_diff>